<commit_message>
multi lib protocol added
</commit_message>
<xml_diff>
--- a/Example_data/pciogreen_pcr-20200414-xr_3.xlsx
+++ b/Example_data/pciogreen_pcr-20200414-xr_3.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\opentrons_protocols\Example_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattstorey/opentrons_protocols/Example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D84390-4320-4FBA-A0C9-878A64AB712D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92884F0-6383-494A-A494-289D6781E228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-8904" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="End point" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -461,7 +463,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1675,60 +1677,60 @@
   <dimension ref="A3:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="L17" sqref="L17:L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.36328125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>1</v>
       </c>
@@ -1766,7 +1768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1802,253 +1804,127 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="3">
-        <v>20000</v>
-      </c>
-      <c r="C17" s="3">
-        <v>20000</v>
-      </c>
-      <c r="D17" s="3">
-        <v>20000</v>
-      </c>
-      <c r="F17" s="3">
-        <v>20000</v>
-      </c>
-      <c r="G17" s="3">
-        <v>20000</v>
-      </c>
-      <c r="H17" s="3">
-        <v>20000</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="3">
-        <v>20000</v>
-      </c>
-      <c r="K17" s="3">
-        <v>20000</v>
-      </c>
-      <c r="L17" s="3">
-        <v>20000</v>
-      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
       <c r="M17" s="6">
         <v>43244</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="3">
-        <v>10000</v>
-      </c>
-      <c r="C18" s="3">
-        <v>10000</v>
-      </c>
-      <c r="D18" s="3">
-        <v>10000</v>
-      </c>
-      <c r="F18" s="3">
-        <v>10000</v>
-      </c>
-      <c r="G18" s="3">
-        <v>10000</v>
-      </c>
-      <c r="H18" s="3">
-        <v>10000</v>
-      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="3">
-        <v>10000</v>
-      </c>
-      <c r="K18" s="3">
-        <v>10000</v>
-      </c>
-      <c r="L18" s="3">
-        <v>10000</v>
-      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="6">
         <v>5330</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="3">
-        <v>5000</v>
-      </c>
-      <c r="C19" s="3">
-        <v>5000</v>
-      </c>
-      <c r="D19" s="3">
-        <v>5000</v>
-      </c>
-      <c r="F19" s="3">
-        <v>5000</v>
-      </c>
-      <c r="G19" s="3">
-        <v>5000</v>
-      </c>
-      <c r="H19" s="3">
-        <v>5000</v>
-      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="3">
-        <v>5000</v>
-      </c>
-      <c r="K19" s="3">
-        <v>5000</v>
-      </c>
-      <c r="L19" s="3">
-        <v>5000</v>
-      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
       <c r="M19" s="6">
         <v>709</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="3">
-        <v>4000</v>
-      </c>
-      <c r="C20" s="3">
-        <v>4000</v>
-      </c>
-      <c r="D20" s="3">
-        <v>4000</v>
-      </c>
-      <c r="F20" s="3">
-        <v>4000</v>
-      </c>
-      <c r="G20" s="3">
-        <v>4000</v>
-      </c>
-      <c r="H20" s="3">
-        <v>4000</v>
-      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="3">
-        <v>4000</v>
-      </c>
-      <c r="K20" s="3">
-        <v>4000</v>
-      </c>
-      <c r="L20" s="3">
-        <v>4000</v>
-      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
       <c r="M20" s="6">
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="3">
-        <v>3000</v>
-      </c>
-      <c r="C21" s="3">
-        <v>3000</v>
-      </c>
-      <c r="D21" s="3">
-        <v>3000</v>
-      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="3">
-        <v>3000</v>
-      </c>
-      <c r="G21" s="3">
-        <v>3000</v>
-      </c>
-      <c r="H21" s="3">
-        <v>3000</v>
-      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="3">
-        <v>3000</v>
-      </c>
-      <c r="K21" s="3">
-        <v>3000</v>
-      </c>
-      <c r="L21" s="3">
-        <v>3000</v>
-      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="3">
-        <v>2000</v>
-      </c>
-      <c r="C22" s="3">
-        <v>2000</v>
-      </c>
-      <c r="D22" s="3">
-        <v>2000</v>
-      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="6"/>
-      <c r="F22" s="3">
-        <v>2000</v>
-      </c>
-      <c r="G22" s="3">
-        <v>2000</v>
-      </c>
-      <c r="H22" s="3">
-        <v>2000</v>
-      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="3">
-        <v>2000</v>
-      </c>
-      <c r="K22" s="3">
-        <v>2000</v>
-      </c>
-      <c r="L22" s="3">
-        <v>2000</v>
-      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
       <c r="M22" s="7"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="3">
-        <v>1000</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1000</v>
-      </c>
-      <c r="D23" s="3">
-        <v>1000</v>
-      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="3">
-        <v>1000</v>
-      </c>
-      <c r="G23" s="3">
-        <v>1000</v>
-      </c>
-      <c r="H23" s="3">
-        <v>1000</v>
-      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="3">
-        <v>1000</v>
-      </c>
-      <c r="K23" s="3">
-        <v>1000</v>
-      </c>
-      <c r="L23" s="3">
-        <v>1000</v>
-      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
       <c r="M23" s="9"/>
     </row>
   </sheetData>
@@ -2065,13 +1941,13 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="2">
         <v>1</v>
       </c>
@@ -2109,7 +1985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -2134,7 +2010,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -2159,7 +2035,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -2184,7 +2060,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2207,7 +2083,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -2232,7 +2108,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -2253,7 +2129,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -2274,7 +2150,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -2295,7 +2171,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>121</v>
       </c>
@@ -2303,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>43244</v>
       </c>
@@ -2311,7 +2187,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>5330</v>
       </c>
@@ -2319,7 +2195,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>709</v>
       </c>
@@ -2327,7 +2203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>186</v>
       </c>
@@ -2335,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11" t="s">
@@ -2352,7 +2228,7 @@
       </c>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>21</v>
       </c>
@@ -2375,7 +2251,7 @@
       </c>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>23</v>
       </c>
@@ -2398,7 +2274,7 @@
       </c>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>25</v>
       </c>
@@ -2421,7 +2297,7 @@
       </c>
       <c r="G21" s="13"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>27</v>
       </c>
@@ -2444,7 +2320,7 @@
       </c>
       <c r="G22" s="13"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>29</v>
       </c>
@@ -2467,7 +2343,7 @@
       </c>
       <c r="G23" s="13"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>31</v>
       </c>
@@ -2490,7 +2366,7 @@
       </c>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>33</v>
       </c>
@@ -2513,7 +2389,7 @@
       </c>
       <c r="G25" s="13"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>35</v>
       </c>
@@ -2536,7 +2412,7 @@
       </c>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>37</v>
       </c>
@@ -2559,7 +2435,7 @@
       </c>
       <c r="G27" s="13"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>39</v>
       </c>
@@ -2582,7 +2458,7 @@
       </c>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>41</v>
       </c>
@@ -2605,7 +2481,7 @@
       </c>
       <c r="G29" s="13"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>43</v>
       </c>
@@ -2628,7 +2504,7 @@
       </c>
       <c r="G30" s="13"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>45</v>
       </c>
@@ -2651,7 +2527,7 @@
       </c>
       <c r="G31" s="13"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>47</v>
       </c>
@@ -2674,7 +2550,7 @@
       </c>
       <c r="G32" s="13"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>49</v>
       </c>
@@ -2697,7 +2573,7 @@
       </c>
       <c r="G33" s="13"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>51</v>
       </c>
@@ -2720,7 +2596,7 @@
       </c>
       <c r="G34" s="13"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>53</v>
       </c>
@@ -2743,7 +2619,7 @@
       </c>
       <c r="G35" s="13"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>55</v>
       </c>
@@ -2768,7 +2644,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>58</v>
       </c>
@@ -2791,7 +2667,7 @@
       </c>
       <c r="G37" s="13"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>60</v>
       </c>
@@ -2814,7 +2690,7 @@
       </c>
       <c r="G38" s="13"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>62</v>
       </c>

</xml_diff>